<commit_message>
Changes after review of Dave
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V1.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V1.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="651">
   <si>
     <t>true</t>
   </si>
@@ -1974,13 +1974,25 @@
   </si>
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
+  </si>
+  <si>
+    <t>Hinweise</t>
+  </si>
+  <si>
+    <t>Für sämtliche Objekte jeder Klasse wird eine UUID erzeugt</t>
+  </si>
+  <si>
+    <t>Die UUID der Objekte der Klasse "AssetItem" ersetzt die InfoGeol-Nr.</t>
+  </si>
+  <si>
+    <t>Die grau hinterlegten rechecke im UML-Diagramm stellen STRUCTUREs dar, die komplexe Datentypen abbilden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2012,6 +2024,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2034,7 +2054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2045,6 +2065,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2069,32 +2093,32 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>458107</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7" name="Gruppieren 6"/>
+        <xdr:cNvPr id="10" name="Gruppieren 9"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4387850" y="44450"/>
-          <a:ext cx="9563100" cy="7524750"/>
-          <a:chOff x="4318000" y="622300"/>
-          <a:chExt cx="9563100" cy="7207250"/>
+          <a:off x="5050971" y="679455"/>
+          <a:ext cx="9561286" cy="8401045"/>
+          <a:chOff x="5157107" y="580571"/>
+          <a:chExt cx="9534071" cy="8190593"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Grafik 1"/>
+          <xdr:cNvPr id="8" name="Grafik 7"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2107,13 +2131,13 @@
               </a:ext>
             </a:extLst>
           </a:blip>
-          <a:srcRect l="7955" t="2880" r="-2777" b="-3680"/>
+          <a:srcRect l="21150"/>
           <a:stretch/>
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4343400" y="717550"/>
-            <a:ext cx="9537700" cy="7112000"/>
+            <a:off x="5309044" y="462648"/>
+            <a:ext cx="9204873" cy="8106561"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2127,8 +2151,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4318000" y="4470400"/>
-            <a:ext cx="9563100" cy="3359150"/>
+            <a:off x="5157107" y="4963338"/>
+            <a:ext cx="9534071" cy="3807826"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2172,8 +2196,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4318000" y="622300"/>
-            <a:ext cx="9563100" cy="3752850"/>
+            <a:off x="5157107" y="601254"/>
+            <a:ext cx="9534071" cy="4254112"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2217,8 +2241,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12179300" y="730250"/>
-            <a:ext cx="1431354" cy="254557"/>
+            <a:off x="12994544" y="723624"/>
+            <a:ext cx="1427009" cy="288558"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2241,7 +2265,7 @@
         </xdr:style>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
+            <a:noAutofit/>
           </a:bodyPr>
           <a:lstStyle/>
           <a:p>
@@ -2276,8 +2300,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12179300" y="4597400"/>
-            <a:ext cx="1666418" cy="254557"/>
+            <a:off x="12994544" y="5107302"/>
+            <a:ext cx="1661360" cy="288558"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2300,7 +2324,7 @@
         </xdr:style>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
+            <a:noAutofit/>
           </a:bodyPr>
           <a:lstStyle/>
           <a:p>
@@ -2600,15 +2624,15 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A4:C8"/>
+  <dimension ref="A4:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
+    <col min="1" max="1" width="44.36328125" customWidth="1"/>
     <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2637,6 +2661,26 @@
       </c>
       <c r="C8" t="s">
         <v>644</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>